<commit_message>
it-180203 fix add sub-level with and without siblings
</commit_message>
<xml_diff>
--- a/dat/mix/issues/2018/2018-02/2018-02-03/issue-tracker.all.20180203_000000.xlsx
+++ b/dat/mix/issues/2018/2018-02/2018-02-03/issue-tracker.all.20180203_000000.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_hierarchy_table" sheetId="10" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="113">
   <si>
     <t>level</t>
   </si>
@@ -1059,8 +1059,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{6132BDFC-AB62-4C4C-A7A3-0498260D18D0}" name="Table110" displayName="Table110" ref="A1:G2" totalsRowShown="0" headerRowCellStyle="HeadingStyle">
-  <autoFilter ref="A1:G2" xr:uid="{0193F43E-A5E8-4CE7-BD2B-3A021D960C2F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{6132BDFC-AB62-4C4C-A7A3-0498260D18D0}" name="Table110" displayName="Table110" ref="A1:G3" totalsRowShown="0" headerRowCellStyle="HeadingStyle">
+  <autoFilter ref="A1:G3" xr:uid="{0193F43E-A5E8-4CE7-BD2B-3A021D960C2F}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{F1E031B2-700E-447F-AE99-70BE424DE5CD}" name="level"/>
     <tableColumn id="2" xr3:uid="{E65603DC-CF03-4CF0-A856-3FD46002FE90}" name="seq"/>
@@ -1577,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC6A9DC5-9969-440D-802A-18F91CA26A23}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1612,7 +1612,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="33" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1632,6 +1632,29 @@
         <v>103</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2141,8 +2164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>